<commit_message>
updated (Now getting stock names in real time  using selenium)
</commit_message>
<xml_diff>
--- a/nifty50_stock_data.xlsx
+++ b/nifty50_stock_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,37 +483,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>₹1,475.80</t>
+          <t>₹514.85</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>₹1,436.65 - ₹1,536.25</t>
+          <t>₹514.10 - ₹533.40</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>₹847.05 - ₹1,536.25</t>
+          <t>₹375.05 - ₹545.90</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>8.37T INR</t>
+          <t>2.76T INR</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9.06M</t>
+          <t>9.84M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>113.20</t>
+          <t>25.56</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.19%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -523,44 +523,44 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>BHARTIARTL</t>
+          <t>WIPRO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>₹1,432.25</t>
+          <t>₹1,430.35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>₹1,426.65 - ₹1,453.00</t>
+          <t>₹1,424.15 - ₹1,464.90</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>₹1,082.30 - ₹1,453.00</t>
+          <t>₹1,082.30 - ₹1,464.90</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.40T INR</t>
+          <t>1.43T INR</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2.16M</t>
+          <t>2.17M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>53.78</t>
+          <t>55.04</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.80%</t>
+          <t>2.73%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -577,37 +577,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>₹1,573.35</t>
+          <t>₹5,385.05</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>₹1,564.25 - ₹1,588.50</t>
+          <t>₹5,352.15 - ₹5,515.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>₹1,281.40 - ₹1,733.00</t>
+          <t>₹4,513.55 - ₹6,442.00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6.49T INR</t>
+          <t>1.59T INR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>9.02M</t>
+          <t>490.57K</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>24.75</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2.43%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -617,44 +617,44 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>INFY</t>
+          <t>LTIM</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>₹3,564.40</t>
+          <t>₹3,904.15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>₹3,538.10 - ₹3,575.95</t>
+          <t>₹3,884.00 - ₹3,978.70</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>₹2,390.05 - ₹3,919.90</t>
+          <t>₹3,214.10 - ₹4,254.75</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4.85T INR</t>
+          <t>14.48T INR</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3.52M</t>
+          <t>2.49M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>37.77</t>
+          <t>31.55</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.79%</t>
+          <t>1.38%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -664,44 +664,44 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>TCS</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>₹1,454.90</t>
+          <t>₹2,473.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>₹1,442.00 - ₹1,468.70</t>
+          <t>₹2,450.10 - ₹2,523.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>₹1,087.05 - ₹1,697.35</t>
+          <t>₹2,172.05 - ₹2,769.65</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.96T INR</t>
+          <t>5.88T INR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.65M</t>
+          <t>2.47M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25.25</t>
+          <t>57.46</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3.56%</t>
+          <t>1.67%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -711,44 +711,44 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>HCLTECH</t>
+          <t>HINDUNILVR</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>₹6,192.50</t>
+          <t>₹2,670.45</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>₹6,145.15 - ₹6,222.50</t>
+          <t>₹2,662.05 - ₹2,723.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>₹4,726.00 - ₹6,874.45</t>
+          <t>₹1,723.86 - ₹2,723.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>912.70B INR</t>
+          <t>1.84T INR</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>440.07K</t>
+          <t>1.07M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>99.01</t>
+          <t>31.77</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.24%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -758,44 +758,44 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>APOLLOHOSP</t>
+          <t>GRASIM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>₹267.50</t>
+          <t>₹1,566.75</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>₹268.35 - ₹275.45</t>
+          <t>₹1,559.50 - ₹1,593.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>₹156.55 - ₹292.95</t>
+          <t>₹1,304.45 - ₹1,733.00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3.45T INR</t>
+          <t>6.61T INR</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>18.72M</t>
+          <t>9.04M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>7.01</t>
+          <t>25.10</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.39%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -805,44 +805,44 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ONGC</t>
+          <t>INFY</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>₹3,934.15</t>
+          <t>₹931.50</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>₹3,897.85 - ₹3,960.00</t>
+          <t>₹931.60 - ₹947.50</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>₹3,193.40 - ₹4,254.75</t>
+          <t>₹723.00 - ₹949.40</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14.13T INR</t>
+          <t>2.33T INR</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.49M</t>
+          <t>2.62M</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>31.03</t>
+          <t>26.07</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1.41%</t>
+          <t>0.77%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -852,44 +852,44 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>TCS</t>
+          <t>JSWSTEEL</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>₹510.80</t>
+          <t>₹2,551.65</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>₹505.85 - ₹516.30</t>
+          <t>₹2,557.00 - ₹2,591.10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>₹375.05 - ₹545.90</t>
+          <t>₹2,145.00 - ₹2,769.30</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.69T INR</t>
+          <t>2.48T INR</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9.68M</t>
+          <t>852.70K</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>24.68</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.19%</t>
+          <t>1.14%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -899,44 +899,44 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>WIPRO</t>
+          <t>NESTLEIND</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>₹1,830.55</t>
+          <t>₹9,501.65</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>₹1,798.90 - ₹1,847.95</t>
+          <t>₹9,505.00 - ₹9,693.95</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>₹1,543.85 - ₹1,987.75</t>
+          <t>₹4,541.00 - ₹10,038.80</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3.55T INR</t>
+          <t>2.66T INR</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7.04M</t>
+          <t>356.96K</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>19.72</t>
+          <t>35.25</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.83%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -946,44 +946,44 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>KOTAKBANK</t>
+          <t>BAJAJ-AUTO</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>₹1,603.10</t>
+          <t>₹5,579.60</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>₹1,583.10 - ₹1,622.00</t>
+          <t>₹5,591.00 - ₹5,728.30</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>₹1,419.05 - ₹1,741.00</t>
+          <t>₹2,835.00 - ₹5,894.55</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.54T INR</t>
+          <t>1.11T INR</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.61M</t>
+          <t>755.88K</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>31.38</t>
+          <t>30.20</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.06%</t>
+          <t>1.95%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -993,44 +993,44 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>BAJAJFINSV</t>
+          <t>HEROMOTOCO</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>₹1,696.15</t>
+          <t>₹174.01</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>₹1,679.00 - ₹1,706.60</t>
+          <t>₹174.01 - ₹175.99</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>₹1,363.55 - ₹1,757.50</t>
+          <t>₹110.40 - ₹184.60</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>12.89T INR</t>
+          <t>2.19T INR</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>21.10M</t>
+          <t>51.10M</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>18.72</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1.16%</t>
+          <t>2.05%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1040,44 +1040,44 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>HDFCBANK</t>
+          <t>TATASTEEL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>₹1,485.50</t>
+          <t>₹1,683.80</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>₹1,445.00 - ₹1,494.00</t>
+          <t>₹1,680.00 - ₹1,702.00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>₹708.00 - ₹1,621.40</t>
+          <t>₹1,363.55 - ₹1,757.50</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3.16T INR</t>
+          <t>13.04T INR</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>8.43M</t>
+          <t>21.19M</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>37.20</t>
+          <t>18.90</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.41%</t>
+          <t>1.15%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1087,44 +1087,44 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ADANIPORTS</t>
+          <t>HDFCBANK</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>₹943.15</t>
+          <t>₹1,459.60</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>₹928.75 - ₹949.40</t>
+          <t>₹1,455.00 - ₹1,473.80</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>₹723.00 - ₹949.40</t>
+          <t>₹1,087.05 - ₹1,697.35</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.27T INR</t>
+          <t>3.97T INR</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2.69M</t>
+          <t>3.73M</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>25.83</t>
+          <t>25.43</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.78%</t>
+          <t>3.53%</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1134,44 +1134,44 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>JSWSTEEL</t>
+          <t>HCLTECH</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>₹425.60</t>
+          <t>₹1,444.05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>₹423.50 - ₹428.00</t>
+          <t>₹1,449.30 - ₹1,466.80</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>₹399.35 - ₹499.70</t>
+          <t>₹847.05 - ₹1,536.25</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5.29T INR</t>
+          <t>8.88T INR</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>16.20M</t>
+          <t>9.81M</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>25.95</t>
+          <t>113.63</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3.24%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1181,44 +1181,44 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>ITC</t>
+          <t>BHARTIARTL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>₹1,480.90</t>
+          <t>₹1,199.60</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>₹1,476.05 - ₹1,492.20</t>
+          <t>₹1,192.05 - ₹1,209.20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>₹996.50 - ₹1,582.00</t>
+          <t>₹899.00 - ₹1,235.00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.20T INR</t>
+          <t>8.64T INR</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.93M</t>
+          <t>19.17M</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>29.07</t>
+          <t>19.51</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.57%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1228,44 +1228,44 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>CIPLA</t>
+          <t>ICICIBANK</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>₹2,888.95</t>
+          <t>₹2,911.50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>₹2,855.00 - ₹2,896.00</t>
+          <t>₹2,902.05 - ₹2,942.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>₹1,390.15 - ₹3,013.50</t>
+          <t>₹1,697.80 - ₹3,059.45</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3.50T INR</t>
+          <t>1.12T INR</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3.91M</t>
+          <t>1.53M</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>28.47</t>
+          <t>14.98</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.74%</t>
+          <t>1.54%</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1275,44 +1275,44 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>M&amp;M</t>
+          <t>SHRIRAMFIN</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>₹3,380.60</t>
+          <t>₹11,667.90</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>₹3,366.35 - ₹3,419.90</t>
+          <t>₹11,667.90 - ₹11,800.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>₹2,882.45 - ₹3,886.95</t>
+          <t>₹7,987.65 - ₹11,874.95</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3.02T INR</t>
+          <t>3.40T INR</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.44M</t>
+          <t>545.37K</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>86.40</t>
+          <t>48.32</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.32%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1322,44 +1322,44 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>TITAN</t>
+          <t>ULTRACEMCO</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>₹593.25</t>
+          <t>₹1,478.10</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>₹590.00 - ₹599.80</t>
+          <t>₹1,471.60 - ₹1,489.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>₹511.40 - ₹710.60</t>
+          <t>₹708.00 - ₹1,621.40</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.28T INR</t>
+          <t>3.23T INR</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5.73M</t>
+          <t>8.75M</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>81.35</t>
+          <t>37.49</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.34%</t>
+          <t>0.40%</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1369,44 +1369,44 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>HDFCLIFE</t>
+          <t>ADANIPORTS</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>₹1,516.25</t>
+          <t>₹303.95</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>₹1,515.60 - ₹1,538.95</t>
+          <t>₹303.30 - ₹306.85</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>₹995.00 - ₹1,638.85</t>
+          <t>₹165.73 - ₹343.98</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3.65T INR</t>
+          <t>1.33T INR</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.91M</t>
+          <t>18.08M</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>38.09</t>
+          <t>4.85</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.89%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1416,44 +1416,44 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>SUNPHARMA</t>
+          <t>BPCL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>₹7,166.75</t>
+          <t>₹1,491.95</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>₹7,105.30 - ₹7,226.00</t>
+          <t>₹1,481.90 - ₹1,503.85</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>₹6,187.80 - ₹8,192.00</t>
+          <t>₹1,251.65 - ₹1,569.40</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4.35T INR</t>
+          <t>1.47T INR</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.11M</t>
+          <t>1.40M</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>30.17</t>
+          <t>79.33</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.51%</t>
+          <t>0.18%</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1463,44 +1463,44 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>BAJFINANCE</t>
+          <t>SBILIFE</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>₹5,430.30</t>
+          <t>₹12,033.85</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>₹5,416.25 - ₹5,490.00</t>
+          <t>₹12,025.00 - ₹12,240.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>₹4,347.70 - ₹5,725.00</t>
+          <t>₹9,254.15 - ₹13,073.95</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.30T INR</t>
+          <t>3.83T INR</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>357.73K</t>
+          <t>542.29K</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>61.40</t>
+          <t>28.14</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.75%</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1510,44 +1510,44 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>BRITANNIA</t>
+          <t>MARUTI</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>₹1,463.45</t>
+          <t>₹7,115.55</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>₹1,450.00 - ₹1,498.80</t>
+          <t>₹7,075.00 - ₹7,159.70</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>₹1,251.65 - ₹1,569.40</t>
+          <t>₹6,187.80 - ₹8,192.00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.49T INR</t>
+          <t>4.44T INR</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.43M</t>
+          <t>1.12M</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>78.89</t>
+          <t>30.23</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.18%</t>
+          <t>0.50%</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1557,44 +1557,44 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>SBILIFE</t>
+          <t>BAJFINANCE</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>₹3,061.10</t>
+          <t>₹595.05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>₹3,062.05 - ₹3,162.00</t>
+          <t>₹589.60 - ₹598.90</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>₹2,220.30 - ₹3,162.00</t>
+          <t>₹511.40 - ₹710.60</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>21.19T INR</t>
+          <t>1.28T INR</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6.84M</t>
+          <t>5.71M</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>30.40</t>
+          <t>81.67</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.33%</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1604,44 +1604,44 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>RELIANCE</t>
+          <t>HDFCLIFE</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>₹4,522.35</t>
+          <t>₹1,480.80</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>₹4,522.35 - ₹4,648.45</t>
+          <t>₹1,475.00 - ₹1,493.70</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>₹3,295.30 - ₹4,648.45</t>
+          <t>₹996.50 - ₹1,582.00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.22T INR</t>
+          <t>1.20T INR</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>635.72K</t>
+          <t>1.88M</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>76.31</t>
+          <t>29.14</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.65%</t>
+          <t>0.57%</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1651,44 +1651,44 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>DIVISLAB</t>
+          <t>CIPLA</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>₹2,462.15</t>
+          <t>₹1,265.25</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>₹2,462.85 - ₹2,490.50</t>
+          <t>₹1,258.85 - ₹1,273.00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>₹2,172.05 - ₹2,769.65</t>
+          <t>₹927.15 - ₹1,310.00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5.78T INR</t>
+          <t>4.00T INR</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2.44M</t>
+          <t>11.15M</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>56.41</t>
+          <t>14.93</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1.70%</t>
+          <t>0.08%</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1698,44 +1698,44 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>HINDUNILVR</t>
+          <t>AXISBANK</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>₹2,880.85</t>
+          <t>₹424.90</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>₹2,862.20 - ₹2,932.00</t>
+          <t>₹424.65 - ₹427.70</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>₹2,670.10 - ₹3,568.00</t>
+          <t>₹399.35 - ₹499.70</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2.79T INR</t>
+          <t>5.32T INR</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.21M</t>
+          <t>16.41M</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>51.22</t>
+          <t>25.98</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1.14%</t>
+          <t>3.23%</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1745,19 +1745,19 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>ASIANPAINT</t>
+          <t>ITC</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>₹685.25</t>
+          <t>₹693.55</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>₹686.00 - ₹697.50</t>
+          <t>₹693.30 - ₹701.85</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1767,17 +1767,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.55T INR</t>
+          <t>1.53T INR</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>9.73M</t>
+          <t>9.76M</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>15.16</t>
+          <t>15.21</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1799,37 +1799,37 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>₹174.16</t>
+          <t>₹6,402.35</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>₹173.57 - ₹177.10</t>
+          <t>₹6,401.20 - ₹6,480.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>₹110.40 - ₹184.60</t>
+          <t>₹5,076.25 - ₹6,505.90</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.17T INR</t>
+          <t>1.04T INR</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>51.15M</t>
+          <t>591.69K</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>19.15</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2.06%</t>
+          <t>0.62%</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1839,44 +1839,44 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>TATASTEEL</t>
+          <t>DRREDDY</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>₹467.05</t>
+          <t>₹3,404.20</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>₹468.00 - ₹476.00</t>
+          <t>₹3,381.50 - ₹3,422.95</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>₹224.15 - ₹527.40</t>
+          <t>₹2,882.45 - ₹3,886.95</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.92T INR</t>
+          <t>3.00T INR</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12.80M</t>
+          <t>1.43M</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>7.80</t>
+          <t>86.53</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.32%</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1886,44 +1886,44 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>COALINDIA</t>
+          <t>TITAN</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>₹1,219.90</t>
+          <t>₹2,866.65</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>₹1,196.35 - ₹1,227.00</t>
+          <t>₹2,838.25 - ₹2,894.05</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>₹899.00 - ₹1,235.00</t>
+          <t>₹1,400.00 - ₹3,013.50</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>8.30T INR</t>
+          <t>3.46T INR</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>19.04M</t>
+          <t>3.66M</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>19.32</t>
+          <t>28.48</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.74%</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1933,44 +1933,44 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>ICICIBANK</t>
+          <t>M&amp;M</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>₹1,288.95</t>
+          <t>₹1,802.50</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>₹1,261.60 - ₹1,289.90</t>
+          <t>₹1,790.00 - ₹1,811.90</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>₹927.15 - ₹1,310.00</t>
+          <t>₹1,543.85 - ₹1,987.75</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3.86T INR</t>
+          <t>3.64T INR</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>11.24M</t>
+          <t>6.88M</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>14.87</t>
+          <t>19.72</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0.08%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1980,46 +1980,46 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>AXISBANK</t>
+          <t>KOTAKBANK</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>₹2,533.75</t>
+          <t>₹274.20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>₹2,528.30 - ₹2,573.70</t>
+          <t>₹272.15 - ₹275.80</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>₹2,145.00 - ₹2,769.30</t>
+          <t>₹158.95 - ₹292.95</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.44T INR</t>
+          <t>3.36T INR</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>837.33K</t>
+          <t>18.99M</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>1.16%</t>
-        </is>
-      </c>
       <c r="H34" t="inlineStr">
         <is>
           <t>NSE</t>
@@ -2027,44 +2027,44 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>NESTLEIND</t>
+          <t>ONGC</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>₹6,235.90</t>
+          <t>₹5,475.55</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>₹6,251.05 - ₹6,420.00</t>
+          <t>₹5,431.05 - ₹5,489.15</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>₹5,004.35 - ₹6,505.90</t>
+          <t>₹4,347.70 - ₹5,725.00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.07T INR</t>
+          <t>1.31T INR</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>577.61K</t>
+          <t>361.03K</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>19.13</t>
+          <t>61.60</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>0.62%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2074,44 +2074,44 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>DRREDDY</t>
+          <t>BRITANNIA</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>₹377.15</t>
+          <t>₹989.75</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>₹376.70 - ₹389.50</t>
+          <t>₹985.20 - ₹997.50</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>₹184.75 - ₹393.20</t>
+          <t>₹584.95 - ₹1,065.60</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3.63T INR</t>
+          <t>3.56T INR</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>19.72M</t>
+          <t>11.14M</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>17.68</t>
+          <t>12.08</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.30%</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2121,44 +2121,44 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>NTPC</t>
+          <t>TATAMOTORS</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>₹9,417.45</t>
+          <t>₹2,917.05</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>₹9,382.25 - ₹9,523.70</t>
+          <t>₹2,888.00 - ₹2,925.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>₹4,541.00 - ₹10,038.80</t>
+          <t>₹2,670.10 - ₹3,568.00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2.71T INR</t>
+          <t>2.76T INR</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>359.84K</t>
+          <t>1.21M</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>34.86</t>
+          <t>51.18</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.84%</t>
+          <t>1.14%</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2168,44 +2168,44 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>BAJAJ-AUTO</t>
+          <t>ASIANPAINT</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>₹4,713.80</t>
+          <t>₹3,177.15</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>₹4,655.30 - ₹4,733.95</t>
+          <t>₹3,161.65 - ₹3,193.15</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>₹3,160.00 - ₹4,976.00</t>
+          <t>₹2,142.00 - ₹3,743.90</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.29T INR</t>
+          <t>3.62T INR</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>573.45K</t>
+          <t>4.05M</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>31.99</t>
+          <t>116.49</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>0.79%</t>
+          <t>0.04%</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2215,44 +2215,44 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>EICHERMOT</t>
+          <t>ADANIENT</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>₹1,502.75</t>
+          <t>₹3,130.80</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>₹1,460.50 - ₹1,491.00</t>
+          <t>₹3,112.20 - ₹3,158.80</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>₹1,316.25 - ₹1,694.50</t>
+          <t>₹2,220.30 - ₹3,162.00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.14T INR</t>
+          <t>20.65T INR</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4.32M</t>
+          <t>7.14M</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>12.70</t>
+          <t>30.35</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1.13%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2262,39 +2262,39 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>INDUSINDBK</t>
+          <t>RELIANCE</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>₹2,637.60</t>
+          <t>₹473.15</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>₹2,587.20 - ₹2,678.95</t>
+          <t>₹471.25 - ₹474.85</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>₹1,723.86 - ₹2,678.95</t>
+          <t>₹226.75 - ₹527.40</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.81T INR</t>
+          <t>2.87T INR</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.06M</t>
+          <t>12.72M</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>31.33</t>
+          <t>7.77</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2309,44 +2309,44 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>GRASIM</t>
+          <t>COALINDIA</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>₹2,951.05</t>
+          <t>₹1,464.50</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>₹2,900.00 - ₹2,969.30</t>
+          <t>₹1,452.95 - ₹1,469.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>₹1,689.15 - ₹3,059.45</t>
+          <t>₹1,337.05 - ₹1,694.50</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.10T INR</t>
+          <t>1.17T INR</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.52M</t>
+          <t>4.41M</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>14.93</t>
+          <t>12.64</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>1.54%</t>
+          <t>1.13%</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2356,44 +2356,44 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>SHRIRAMFIN</t>
+          <t>INDUSINDBK</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>₹844.00</t>
+          <t>₹1,588.15</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>₹844.00 - ₹864.00</t>
+          <t>₹1,578.00 - ₹1,590.95</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>₹543.20 - ₹912.00</t>
+          <t>₹1,419.05 - ₹1,741.00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7.57T INR</t>
+          <t>2.54T INR</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>23.53M</t>
+          <t>1.66M</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>11.29</t>
+          <t>31.23</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1.61%</t>
+          <t>0.06%</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2403,44 +2403,44 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>SBIN</t>
+          <t>BAJAJFINSV</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>₹331.55</t>
+          <t>₹4,672.95</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>₹329.60 - ₹337.35</t>
+          <t>₹4,626.00 - ₹4,729.45</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>₹177.53 - ₹348.70</t>
+          <t>₹3,160.00 - ₹4,976.00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3.09T INR</t>
+          <t>1.29T INR</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>22.05M</t>
+          <t>595.17K</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>19.79</t>
+          <t>31.91</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.79%</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2450,44 +2450,44 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>POWERGRID</t>
+          <t>EICHERMOT</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>₹972.10</t>
+          <t>₹848.95</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>₹972.55 - ₹998.50</t>
+          <t>₹842.05 - ₹850.50</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>₹575.50 - ₹1,065.60</t>
+          <t>₹543.20 - ₹912.00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3.63T INR</t>
+          <t>7.52T INR</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10.81M</t>
+          <t>23.90M</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>12.08</t>
+          <t>11.22</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>0.30%</t>
+          <t>1.62%</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2497,44 +2497,44 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>TATAMOTORS</t>
+          <t>SBIN</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>₹12,178.75</t>
+          <t>₹1,097.45</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>₹12,004.15 - ₹12,201.50</t>
+          <t>₹1,088.30 - ₹1,097.45</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>₹9,254.15 - ₹13,073.95</t>
+          <t>₹822.00 - ₹1,269.00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3.75T INR</t>
+          <t>1.03T INR</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>530.58K</t>
+          <t>1.69M</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>28.03</t>
+          <t>88.44</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>0.75%</t>
+          <t>0.71%</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2544,44 +2544,44 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>TATACONSUM</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>₹1,085.60</t>
+          <t>₹330.95</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>₹1,085.00 - ₹1,104.00</t>
+          <t>₹325.25 - ₹331.75</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>₹822.00 - ₹1,269.00</t>
+          <t>₹177.53 - ₹348.70</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.05T INR</t>
+          <t>3.06T INR</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.69M</t>
+          <t>22.47M</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>89.17</t>
+          <t>19.64</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0.71%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2591,44 +2591,44 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TATACONSUM</t>
+          <t>POWERGRID</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>₹11,716.70</t>
+          <t>₹3,548.45</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>₹11,469.85 - ₹11,779.00</t>
+          <t>₹3,514.00 - ₹3,541.40</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>₹7,987.65 - ₹11,874.95</t>
+          <t>₹2,415.05 - ₹3,919.90</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3.36T INR</t>
+          <t>4.86T INR</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>532.01K</t>
+          <t>3.53M</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>47.97</t>
+          <t>37.49</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.80%</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2638,44 +2638,44 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>ULTRACEMCO</t>
+          <t>LT</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>₹3,175.15</t>
+          <t>₹4,596.45</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>₹3,157.00 - ₹3,211.95</t>
+          <t>₹4,540.20 - ₹4,606.45</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>₹2,142.00 - ₹3,743.90</t>
+          <t>₹3,295.30 - ₹4,648.45</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3.62T INR</t>
+          <t>1.19T INR</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>4.05M</t>
+          <t>639.85K</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>116.56</t>
+          <t>75.54</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>0.04%</t>
+          <t>0.66%</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2685,44 +2685,44 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>ADANIENT</t>
+          <t>DIVISLAB</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>₹5,485.20</t>
+          <t>₹1,520.85</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>₹5,452.10 - ₹5,605.25</t>
+          <t>₹1,503.85 - ₹1,530.00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>₹2,795.00 - ₹5,894.55</t>
+          <t>₹1,020.05 - ₹1,638.85</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.13T INR</t>
+          <t>3.60T INR</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>758.21K</t>
+          <t>2.95M</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>29.89</t>
+          <t>37.78</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>1.97%</t>
+          <t>0.90%</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2732,7 +2732,101 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>HEROMOTOCO</t>
+          <t>SUNPHARMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>₹6,185.70</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>₹6,108.45 - ₹6,180.00</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>₹4,726.00 - ₹6,874.45</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>881.38B INR</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>442.30K</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>97.97</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>0.24%</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>APOLLOHOSP</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>₹378.35</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>₹367.80 - ₹382.00</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>₹184.75 - ₹393.20</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>3.60T INR</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>20.27M</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>17.34</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>NTPC</t>
         </is>
       </c>
     </row>

</xml_diff>